<commit_message>
did not fix issue with CO2 embodied in hot metal
</commit_message>
<xml_diff>
--- a/data/steel/steel_IEAGHG_calcs-CONTRIBUTION.xlsx
+++ b/data/steel/steel_IEAGHG_calcs-CONTRIBUTION.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F0A069-F0D1-4F4B-A7F1-F31546CBB770}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke Oven" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="181">
   <si>
     <t>CaCO3</t>
   </si>
@@ -564,15 +565,25 @@
   </si>
   <si>
     <t>emissions</t>
+  </si>
+  <si>
+    <t>CO2__embodied in hot metal (subtract from BF emissions)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -655,14 +666,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -760,6 +772,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -795,6 +824,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -970,25 +1016,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1017,7 +1063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1037,7 +1083,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>153</v>
       </c>
@@ -1057,7 +1103,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>153</v>
       </c>
@@ -1080,7 +1126,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>153</v>
       </c>
@@ -1103,7 +1149,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1126,7 +1172,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>154</v>
       </c>
@@ -1149,7 +1195,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>153</v>
       </c>
@@ -1172,7 +1218,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>155</v>
       </c>
@@ -1193,7 +1239,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1216,7 +1262,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1285,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -1266,7 +1312,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1277,7 +1323,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1295,25 +1341,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -1345,7 +1391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -1368,7 +1414,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -1388,7 +1434,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1411,7 +1457,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1431,7 +1477,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1451,7 +1497,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1471,7 +1517,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1494,7 +1540,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -1517,7 +1563,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -1540,7 +1586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -1566,7 +1612,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -1592,7 +1638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -1615,7 +1661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -1642,7 +1688,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -1665,7 +1711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -1688,7 +1734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -1711,7 +1757,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -1734,7 +1780,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1757,7 +1803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -1780,7 +1826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -1803,7 +1849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1826,7 +1872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1849,7 +1895,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1872,7 +1918,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -1901,7 +1947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -1934,26 +1980,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33:I33"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1985,7 +2031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -2011,7 +2057,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -2037,7 +2083,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -2063,7 +2109,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -2089,7 +2135,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -2113,7 +2159,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -2137,7 +2183,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -2163,7 +2209,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -2189,7 +2235,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -2215,7 +2261,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -2241,7 +2287,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -2269,7 +2315,7 @@
       </c>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -2293,7 +2339,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -2317,7 +2363,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -2341,7 +2387,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -2365,7 +2411,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -2389,7 +2435,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -2413,7 +2459,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -2441,7 +2487,7 @@
       </c>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -2467,7 +2513,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -2493,7 +2539,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -2521,7 +2567,7 @@
       </c>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2549,7 +2595,7 @@
       </c>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -2575,7 +2621,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -2601,7 +2647,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -2625,7 +2671,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -2649,7 +2695,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -2673,7 +2719,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -2699,7 +2745,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2725,7 +2771,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>175</v>
       </c>
@@ -2751,7 +2797,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>175</v>
       </c>
@@ -2761,8 +2807,8 @@
       <c r="C32" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>176</v>
+      <c r="D32" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>17</v>
@@ -2775,7 +2821,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>175</v>
       </c>
@@ -2803,7 +2849,7 @@
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>128</v>
       </c>
@@ -2829,7 +2875,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -2855,7 +2901,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>128</v>
       </c>
@@ -2879,7 +2925,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -2903,7 +2949,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -2929,7 +2975,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>128</v>
       </c>
@@ -2955,7 +3001,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>128</v>
       </c>
@@ -2983,7 +3029,7 @@
       </c>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>128</v>
       </c>
@@ -3009,7 +3055,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>128</v>
       </c>
@@ -3037,7 +3083,7 @@
       </c>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>128</v>
       </c>
@@ -3065,7 +3111,7 @@
       </c>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>128</v>
       </c>
@@ -3091,7 +3137,7 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>128</v>
       </c>
@@ -3118,7 +3164,7 @@
       </c>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -3145,7 +3191,7 @@
       </c>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -3171,7 +3217,7 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>128</v>
       </c>
@@ -3198,7 +3244,7 @@
       </c>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>128</v>
       </c>
@@ -3225,7 +3271,7 @@
       </c>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>128</v>
       </c>
@@ -3251,7 +3297,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -3261,7 +3307,7 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -3279,25 +3325,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -3329,7 +3375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>127</v>
       </c>
@@ -3352,7 +3398,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>127</v>
       </c>
@@ -3375,7 +3421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>127</v>
       </c>
@@ -3398,7 +3444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>89</v>
       </c>
@@ -3421,7 +3467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>89</v>
       </c>
@@ -3444,7 +3490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>89</v>
       </c>
@@ -3467,7 +3513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>89</v>
       </c>
@@ -3490,7 +3536,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>89</v>
       </c>
@@ -3516,7 +3562,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -3539,7 +3585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>88</v>
       </c>
@@ -3562,7 +3608,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>88</v>
       </c>
@@ -3582,7 +3628,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>88</v>
       </c>
@@ -3602,7 +3648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>90</v>
       </c>
@@ -3625,7 +3671,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>90</v>
       </c>
@@ -3648,7 +3694,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>90</v>
       </c>
@@ -3671,7 +3717,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>128</v>
       </c>
@@ -3697,7 +3743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>128</v>
       </c>
@@ -3723,7 +3769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>128</v>
       </c>
@@ -3755,21 +3801,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>87</v>
       </c>
@@ -3801,7 +3847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -3824,7 +3870,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -3847,7 +3893,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -3873,7 +3919,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -3896,7 +3942,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3922,7 +3968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -3945,7 +3991,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -3968,7 +4014,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -3994,7 +4040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -4020,7 +4066,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4043,7 +4089,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -4066,7 +4112,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -4089,7 +4135,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -4112,7 +4158,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -4147,24 +4193,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>87</v>
       </c>
@@ -4196,7 +4242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -4219,7 +4265,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -4242,7 +4288,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -4265,7 +4311,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -4291,7 +4337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -4314,7 +4360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -4337,7 +4383,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>88</v>
       </c>

</xml_diff>